<commit_message>
Upload FoICStCT and BHNVEAL plus a few corrections
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSDbS/BAU RPS Data by Subregion.xlsx
+++ b/InputData/elec/BRPSDbS/BAU RPS Data by Subregion.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\elec\BRPSDbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\elec\BRPSDbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC89E7B-D04C-4D53-A4DB-EEA128A78EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136E545D-F7E5-4E1E-A55A-780FE2FC056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="13830" windowHeight="15060" tabRatio="722" firstSheet="3" activeTab="4" xr2:uid="{AC72C5EC-EE21-41F5-88E2-B69BAFE27B97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="722" firstSheet="3" activeTab="3" xr2:uid="{AC72C5EC-EE21-41F5-88E2-B69BAFE27B97}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Electricity generation EU" sheetId="5" r:id="rId2"/>
     <sheet name="BRPSPTY" sheetId="2" r:id="rId3"/>
-    <sheet name="BRPSDbS-RPS-percentage" sheetId="3" r:id="rId4"/>
+    <sheet name="BRPSDbS-RPS-percentages" sheetId="3" r:id="rId4"/>
     <sheet name="BRPSDbS-electricity-shares" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -1101,32 +1101,32 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="45.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="45.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -1146,82 +1146,82 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="8"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="9"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
@@ -1243,9 +1243,9 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>2.1797101449275366E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>3.6096618357487932E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1.8125603864734302E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>5.4106280193236727E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>1.739130434782609E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>3.0647342995169087E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>2.2801932367149764E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>1.2599033816425123E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.19791304347826091</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>2.461835748792271E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>0.19516908212560391</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>1.5768115942028989E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1.2328502415458938E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>9.0434782608695662E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>9.7004830917874416E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>2.1642512077294689E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>1.6231884057971019E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>1.1594202898550727E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3.7874396135265706E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>6.2415458937198076E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>1.8086956521739132E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>2.2299516908212566E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>1.1285024154589374E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>5.6425120772946868E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>9.5536231884057979E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>6.2415458937198076E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>42</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>43</v>
       </c>
@@ -1618,12 +1618,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1831,16 +1831,16 @@
   </sheetPr>
   <dimension ref="A1:CD61"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -9342,7 +9342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -10117,7 +10117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -10613,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -10861,7 +10861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -11357,7 +11357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -11853,7 +11853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -12349,7 +12349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -12597,7 +12597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -12845,7 +12845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -13093,7 +13093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -13341,7 +13341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>143</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -14085,7 +14085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -14581,7 +14581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -14829,7 +14829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -15077,7 +15077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -15325,7 +15325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>151</v>
       </c>
@@ -15573,7 +15573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>152</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -16069,7 +16069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>154</v>
       </c>
@@ -16317,7 +16317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>155</v>
       </c>
@@ -16565,7 +16565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>156</v>
       </c>
@@ -16813,7 +16813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>157</v>
       </c>
@@ -17061,7 +17061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -17309,7 +17309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -17557,7 +17557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>160</v>
       </c>
@@ -17818,13 +17818,13 @@
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>161</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -17841,7 +17841,7 @@
         <v>2.1797101449275366E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -17850,7 +17850,7 @@
         <v>3.6096618357487932E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -17859,7 +17859,7 @@
         <v>1.8125603864734302E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -17868,7 +17868,7 @@
         <v>5.4106280193236727E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -17877,7 +17877,7 @@
         <v>1.739130434782609E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -17886,7 +17886,7 @@
         <v>3.0647342995169087E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -17895,7 +17895,7 @@
         <v>2.2801932367149764E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -17904,7 +17904,7 @@
         <v>1.2599033816425123E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -17913,7 +17913,7 @@
         <v>0.19791304347826091</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -17922,7 +17922,7 @@
         <v>2.461835748792271E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -17931,7 +17931,7 @@
         <v>0.19516908212560391</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -17940,7 +17940,7 @@
         <v>1.5768115942028989E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -17949,7 +17949,7 @@
         <v>1.2328502415458938E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -17958,7 +17958,7 @@
         <v>9.0434782608695662E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -17967,7 +17967,7 @@
         <v>9.7004830917874416E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -17976,7 +17976,7 @@
         <v>2.1642512077294689E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -17985,7 +17985,7 @@
         <v>1.6231884057971019E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>1.1594202898550727E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -18003,7 +18003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -18012,7 +18012,7 @@
         <v>3.7874396135265706E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -18021,7 +18021,7 @@
         <v>6.2415458937198076E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -18030,7 +18030,7 @@
         <v>1.8086956521739132E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -18039,7 +18039,7 @@
         <v>2.2299516908212566E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -18048,7 +18048,7 @@
         <v>1.1285024154589374E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -18057,7 +18057,7 @@
         <v>5.6425120772946868E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -18066,7 +18066,7 @@
         <v>9.5536231884057979E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -18075,7 +18075,7 @@
         <v>6.2415458937198076E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -18091,7 +18091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -18099,7 +18099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -18107,7 +18107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -18115,7 +18115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -18123,7 +18123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -18131,7 +18131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -18139,7 +18139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -18147,7 +18147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -18155,7 +18155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -18163,7 +18163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -18171,7 +18171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -18179,7 +18179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -18187,7 +18187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -18195,7 +18195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>143</v>
       </c>
@@ -18203,7 +18203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -18211,7 +18211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -18219,7 +18219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -18227,7 +18227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -18235,7 +18235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -18243,7 +18243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -18251,7 +18251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -18259,7 +18259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>151</v>
       </c>
@@ -18267,7 +18267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>152</v>
       </c>
@@ -18275,7 +18275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -18283,7 +18283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>154</v>
       </c>
@@ -18291,7 +18291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>155</v>
       </c>
@@ -18299,7 +18299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>156</v>
       </c>
@@ -18307,7 +18307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>157</v>
       </c>
@@ -18315,7 +18315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>159</v>
       </c>
@@ -18331,7 +18331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>160</v>
       </c>
@@ -18345,6 +18345,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -18573,27 +18593,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9840284-0176-400F-B9D9-6563EC99BFC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83B7572D-F31B-4B49-899C-A72CB6F7CF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E667D2-0F1C-4E1F-8A69-88295E72108D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18610,23 +18629,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83B7572D-F31B-4B49-899C-A72CB6F7CF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9840284-0176-400F-B9D9-6563EC99BFC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes RQSD and removes BAU RPS
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSDbS/BAU RPS Data by Subregion.xlsx
+++ b/InputData/elec/BRPSDbS/BAU RPS Data by Subregion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\elec\BRPSDbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BRPSDbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136E545D-F7E5-4E1E-A55A-780FE2FC056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C90A27C-57B7-4576-B610-2DF7674887A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="722" firstSheet="3" activeTab="3" xr2:uid="{AC72C5EC-EE21-41F5-88E2-B69BAFE27B97}"/>
+    <workbookView xWindow="35880" yWindow="4050" windowWidth="19185" windowHeight="11265" tabRatio="722" activeTab="3" xr2:uid="{AC72C5EC-EE21-41F5-88E2-B69BAFE27B97}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -798,9 +798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -838,7 +838,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -944,7 +944,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1086,7 +1086,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1097,8 +1097,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B10:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,7 +1239,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1831,8 +1831,8 @@
   </sheetPr>
   <dimension ref="A1:CD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2093,128 +2093,97 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -2372,128 +2341,97 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -2651,128 +2589,97 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC4">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -2930,128 +2837,97 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -3209,128 +3085,97 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -3488,128 +3333,97 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z7">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -3767,128 +3581,97 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC8">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -4046,128 +3829,97 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y9">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF9">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG9">
         <v>0</v>
@@ -4325,128 +4077,97 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z10">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB10">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD10">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG10">
         <v>0</v>
@@ -4604,128 +4325,97 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y11">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z11">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA11">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB11">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG11">
         <v>0</v>
@@ -4883,128 +4573,97 @@
         <v>24</v>
       </c>
       <c r="B12">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y12">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z12">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA12">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB12">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC12">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD12">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE12">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF12">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>0</v>
@@ -5162,128 +4821,97 @@
         <v>25</v>
       </c>
       <c r="B13">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X13">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y13">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z13">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA13">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB13">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC13">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD13">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE13">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF13">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG13">
         <v>0</v>
@@ -5441,128 +5069,97 @@
         <v>26</v>
       </c>
       <c r="B14">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA14">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD14">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -5720,128 +5317,97 @@
         <v>27</v>
       </c>
       <c r="B15">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF15">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG15">
         <v>0</v>
@@ -5999,128 +5565,97 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y16">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z16">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA16">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB16">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC16">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD16">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE16">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF16">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG16">
         <v>0</v>
@@ -6278,128 +5813,97 @@
         <v>29</v>
       </c>
       <c r="B17">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y17">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z17">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA17">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB17">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC17">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF17">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG17">
         <v>0</v>
@@ -6557,128 +6061,97 @@
         <v>30</v>
       </c>
       <c r="B18">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y18">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z18">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA18">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB18">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC18">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD18">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE18">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF18">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG18">
         <v>0</v>
@@ -6836,128 +6309,97 @@
         <v>31</v>
       </c>
       <c r="B19">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U19">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V19">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X19">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y19">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z19">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA19">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB19">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC19">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD19">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE19">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF19">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -7115,128 +6557,97 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X20">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y20">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z20">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA20">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB20">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC20">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD20">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE20">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF20">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG20">
         <v>0</v>
@@ -7394,128 +6805,97 @@
         <v>34</v>
       </c>
       <c r="B21">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T21">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U21">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V21">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X21">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y21">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z21">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA21">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB21">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC21">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD21">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE21">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF21">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG21">
         <v>0</v>
@@ -7673,128 +7053,97 @@
         <v>35</v>
       </c>
       <c r="B22">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V22">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W22">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X22">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y22">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA22">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB22">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE22">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF22">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG22">
         <v>0</v>
@@ -7952,128 +7301,97 @@
         <v>36</v>
       </c>
       <c r="B23">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O23">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q23">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R23">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T23">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U23">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V23">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W23">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X23">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y23">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z23">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA23">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB23">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC23">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD23">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE23">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF23">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG23">
         <v>0</v>
@@ -8231,128 +7549,97 @@
         <v>37</v>
       </c>
       <c r="B24">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O24">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P24">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q24">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R24">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S24">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T24">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U24">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V24">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W24">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X24">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y24">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z24">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA24">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB24">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC24">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD24">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE24">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF24">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG24">
         <v>0</v>
@@ -8510,128 +7797,97 @@
         <v>38</v>
       </c>
       <c r="B25">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L25">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O25">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U25">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V25">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X25">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y25">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z25">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA25">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB25">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC25">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD25">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE25">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF25">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG25">
         <v>0</v>
@@ -8789,128 +8045,97 @@
         <v>39</v>
       </c>
       <c r="B26">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L26">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T26">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U26">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V26">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W26">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X26">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y26">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z26">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA26">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB26">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC26">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD26">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE26">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF26">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <v>0</v>
@@ -9068,128 +8293,97 @@
         <v>40</v>
       </c>
       <c r="B27">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O27">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V27">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y27">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z27">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA27">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB27">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD27">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE27">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF27">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG27">
         <v>0</v>
@@ -9347,128 +8541,97 @@
         <v>41</v>
       </c>
       <c r="B28">
-        <f>BRPSPTY!B$2</f>
-        <v>0.39912416911933146</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <f>BRPSPTY!C$2</f>
-        <v>0.38847727423831385</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <f>BRPSPTY!D$2</f>
-        <v>0.40678144979051944</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <f>BRPSPTY!E$2</f>
-        <v>0.41710855978319605</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <f>BRPSPTY!F$2</f>
-        <v>0.42743566977587272</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <f>BRPSPTY!G$2</f>
-        <v>0.43776277976854933</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <f>BRPSPTY!H$2</f>
-        <v>0.44392189315073527</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <f>BRPSPTY!I$2</f>
-        <v>0.45008100653292127</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <f>BRPSPTY!J$2</f>
-        <v>0.45624011991510721</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <f>BRPSPTY!K$2</f>
-        <v>0.46239923329729321</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <f>BRPSPTY!L$2</f>
-        <v>0.46855834667947915</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <f>BRPSPTY!M$2</f>
-        <v>0.47822621893375017</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <f>BRPSPTY!N$2</f>
-        <v>0.48789409118802118</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <f>BRPSPTY!O$2</f>
-        <v>0.4975619634422922</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <f>BRPSPTY!P$2</f>
-        <v>0.50722983569656321</v>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <f>BRPSPTY!Q$2</f>
-        <v>0.51689770795083423</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <f>BRPSPTY!R$2</f>
-        <v>0.52600669989761895</v>
+        <v>0</v>
       </c>
       <c r="S28">
-        <f>BRPSPTY!S$2</f>
-        <v>0.53511569184440366</v>
+        <v>0</v>
       </c>
       <c r="T28">
-        <f>BRPSPTY!T$2</f>
-        <v>0.54422468379118827</v>
+        <v>0</v>
       </c>
       <c r="U28">
-        <f>BRPSPTY!U$2</f>
-        <v>0.55333367573797299</v>
+        <v>0</v>
       </c>
       <c r="V28">
-        <f>BRPSPTY!V$2</f>
-        <v>0.5624426676847577</v>
+        <v>0</v>
       </c>
       <c r="W28">
-        <f>BRPSPTY!W$2</f>
-        <v>0.57115389074898182</v>
+        <v>0</v>
       </c>
       <c r="X28">
-        <f>BRPSPTY!X$2</f>
-        <v>0.57986511381320593</v>
+        <v>0</v>
       </c>
       <c r="Y28">
-        <f>BRPSPTY!Y$2</f>
-        <v>0.58857633687742994</v>
+        <v>0</v>
       </c>
       <c r="Z28">
-        <f>BRPSPTY!Z$2</f>
-        <v>0.59728755994165406</v>
+        <v>0</v>
       </c>
       <c r="AA28">
-        <f>BRPSPTY!AA$2</f>
-        <v>0.60599878300587817</v>
+        <v>0</v>
       </c>
       <c r="AB28">
-        <f>BRPSPTY!AB$2</f>
-        <v>0.61464409535256004</v>
+        <v>0</v>
       </c>
       <c r="AC28">
-        <f>BRPSPTY!AC$2</f>
-        <v>0.62328940769924179</v>
+        <v>0</v>
       </c>
       <c r="AD28">
-        <f>BRPSPTY!AD$2</f>
-        <v>0.63193472004592366</v>
+        <v>0</v>
       </c>
       <c r="AE28">
-        <f>BRPSPTY!AE$2</f>
-        <v>0.64058003239260541</v>
+        <v>0</v>
       </c>
       <c r="AF28">
-        <f>BRPSPTY!AF$2</f>
-        <v>0.64922534473928728</v>
+        <v>0</v>
       </c>
       <c r="AG28">
         <v>0</v>
@@ -17818,8 +16981,8 @@
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18345,26 +17508,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -18593,10 +17736,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9840284-0176-400F-B9D9-6563EC99BFC2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E667D2-0F1C-4E1F-8A69-88295E72108D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18613,20 +17787,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E667D2-0F1C-4E1F-8A69-88295E72108D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9840284-0176-400F-B9D9-6563EC99BFC2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>